<commit_message>
Tax Bill Configuration Step Definition Update
</commit_message>
<xml_diff>
--- a/src/test/resources/Sheet/Configsheet.xlsx
+++ b/src/test/resources/Sheet/Configsheet.xlsx
@@ -3,22 +3,23 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jones\eclipse-workspace\Automation-QaPlateron\src\test\resources\Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A75D8027-F1B0-4B22-968B-E4B6C2788876}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{509CF12C-ED98-485F-9C47-4F52F13F8321}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="23280" windowHeight="12480" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Employee Details" r:id="rId5" sheetId="2"/>
+    <sheet name="Bill Configuration" sheetId="3" r:id="rId2"/>
+    <sheet name="Employee Details" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="92">
   <si>
     <t>Employee Name</t>
   </si>
@@ -35,14 +36,280 @@
   </si>
   <si>
     <t>PIN</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>PhoneNo</t>
+  </si>
+  <si>
+    <t>TEst Test</t>
+  </si>
+  <si>
+    <t>Owner</t>
+  </si>
+  <si>
+    <t>2092</t>
+  </si>
+  <si>
+    <t>test+1@gmail.com</t>
+  </si>
+  <si>
+    <t>+1 (222) 222 - 2222</t>
+  </si>
+  <si>
+    <t>Auto14</t>
+  </si>
+  <si>
+    <t>Waiter</t>
+  </si>
+  <si>
+    <t>5201</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>+1 (823) 445 - 7120</t>
+  </si>
+  <si>
+    <t>Auto15</t>
+  </si>
+  <si>
+    <t>Busser</t>
+  </si>
+  <si>
+    <t>5389</t>
+  </si>
+  <si>
+    <t>+1 (923) 445 - 7120</t>
+  </si>
+  <si>
+    <t>Auto3</t>
+  </si>
+  <si>
+    <t>4824</t>
+  </si>
+  <si>
+    <t>+1 (723) 115 - 7110</t>
+  </si>
+  <si>
+    <t>Auto4</t>
+  </si>
+  <si>
+    <t>9853</t>
+  </si>
+  <si>
+    <t>+1 (823) 115 - 7110</t>
+  </si>
+  <si>
+    <t>Auto5</t>
+  </si>
+  <si>
+    <t>2114</t>
+  </si>
+  <si>
+    <t>+1 (923) 115 - 7110</t>
+  </si>
+  <si>
+    <t>AutTest34</t>
+  </si>
+  <si>
+    <t>Manager</t>
+  </si>
+  <si>
+    <t>9694</t>
+  </si>
+  <si>
+    <t>+1 (235) 512 - 3330</t>
+  </si>
+  <si>
+    <t>7298</t>
+  </si>
+  <si>
+    <t>+1 (245) 541 - 3331</t>
+  </si>
+  <si>
+    <t>9185</t>
+  </si>
+  <si>
+    <t>+1 (235) 512 - 3320</t>
+  </si>
+  <si>
+    <t>Test34</t>
+  </si>
+  <si>
+    <t>1771</t>
+  </si>
+  <si>
+    <t>+1 (245) 541 - 1110</t>
+  </si>
+  <si>
+    <t>tester</t>
+  </si>
+  <si>
+    <t>8761</t>
+  </si>
+  <si>
+    <t>+1 (098) 765 - 4323</t>
+  </si>
+  <si>
+    <t>testy</t>
+  </si>
+  <si>
+    <t>4687</t>
+  </si>
+  <si>
+    <t>+1 (087) 654 - 3245</t>
+  </si>
+  <si>
+    <t>uto11</t>
+  </si>
+  <si>
+    <t>8894</t>
+  </si>
+  <si>
+    <t>+1 (523) 445 - 7190</t>
+  </si>
+  <si>
+    <t>uto12</t>
+  </si>
+  <si>
+    <t>3381</t>
+  </si>
+  <si>
+    <t>+1 (623) 445 - 7190</t>
+  </si>
+  <si>
+    <t>uto13</t>
+  </si>
+  <si>
+    <t>6545</t>
+  </si>
+  <si>
+    <t>+1 (723) 445 - 7190</t>
+  </si>
+  <si>
+    <t>uto14</t>
+  </si>
+  <si>
+    <t>8054</t>
+  </si>
+  <si>
+    <t>+1 (823) 445 - 7190</t>
+  </si>
+  <si>
+    <t>uto15</t>
+  </si>
+  <si>
+    <t>7381</t>
+  </si>
+  <si>
+    <t>+1 (923) 445 - 7190</t>
+  </si>
+  <si>
+    <t>y1</t>
+  </si>
+  <si>
+    <t>4705</t>
+  </si>
+  <si>
+    <t>+1 (523) 445 - 7210</t>
+  </si>
+  <si>
+    <t>y2</t>
+  </si>
+  <si>
+    <t>6012</t>
+  </si>
+  <si>
+    <t>+1 (623) 445 - 7210</t>
+  </si>
+  <si>
+    <t>y3</t>
+  </si>
+  <si>
+    <t>3905</t>
+  </si>
+  <si>
+    <t>+1 (723) 445 - 7210</t>
+  </si>
+  <si>
+    <t>y4</t>
+  </si>
+  <si>
+    <t>7670</t>
+  </si>
+  <si>
+    <t>+1 (823) 445 - 7210</t>
+  </si>
+  <si>
+    <t>y5</t>
+  </si>
+  <si>
+    <t>8799</t>
+  </si>
+  <si>
+    <t>+1 (923) 445 - 7210</t>
+  </si>
+  <si>
+    <t>Sales Tax</t>
+  </si>
+  <si>
+    <t>Apply sales tax on the subtotal after deductions</t>
+  </si>
+  <si>
+    <t>Apply sales tax on the tip after deductions</t>
+  </si>
+  <si>
+    <t>Service Fee Percentage</t>
+  </si>
+  <si>
+    <t>Service Fee Percentage inclusive of sales tax</t>
+  </si>
+  <si>
+    <t>Service Fee Tax Percentage</t>
+  </si>
+  <si>
+    <t>Apply service fee on the subtotal after deductions</t>
+  </si>
+  <si>
+    <t>Gratuity Enable</t>
+  </si>
+  <si>
+    <t>Gratuity Based on (Guest Count / Order Amount)</t>
+  </si>
+  <si>
+    <t>Gratuity percentage</t>
+  </si>
+  <si>
+    <t>Guest count reaches this No</t>
+  </si>
+  <si>
+    <t>subtotal reaches this amount</t>
+  </si>
+  <si>
+    <t>Gratuity Tax percentage</t>
+  </si>
+  <si>
+    <t>Apply Gratuity for TakeAway</t>
+  </si>
+  <si>
+    <t>Apply Gratuity for Dine-In</t>
+  </si>
+  <si>
+    <t>Apply gratuity on the subtotal after deductions</t>
+  </si>
+  <si>
+    <t>Value</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -51,15 +318,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -67,12 +340,38 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -355,7 +654,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
@@ -364,14 +663,155 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09244190-151A-43A4-A916-8BD3607753C8}">
+  <dimension ref="A1:B17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="48.5703125" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" style="5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1"/>
+      <c r="B1" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B2" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B3" s="4"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B4" s="4"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B5" s="4"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B6" s="4"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B7" s="4"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B8" s="4"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B9" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B10" s="4">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B11" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B12" s="4">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B13" s="4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B14" s="4">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B15" s="4">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B16" s="4">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B17" s="4">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -381,8 +821,388 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" t="s">
+        <v>40</v>
+      </c>
+      <c r="D12" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" t="s">
+        <v>43</v>
+      </c>
+      <c r="D13" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D14" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>48</v>
+      </c>
+      <c r="B15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" t="s">
+        <v>49</v>
+      </c>
+      <c r="D15" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>51</v>
+      </c>
+      <c r="B16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" t="s">
+        <v>52</v>
+      </c>
+      <c r="D16" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>54</v>
+      </c>
+      <c r="B17" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" t="s">
+        <v>55</v>
+      </c>
+      <c r="D17" t="s">
+        <v>13</v>
+      </c>
+      <c r="E17" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>57</v>
+      </c>
+      <c r="B18" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" t="s">
+        <v>58</v>
+      </c>
+      <c r="D18" t="s">
+        <v>13</v>
+      </c>
+      <c r="E18" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>60</v>
+      </c>
+      <c r="B19" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" t="s">
+        <v>61</v>
+      </c>
+      <c r="D19" t="s">
+        <v>13</v>
+      </c>
+      <c r="E19" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>63</v>
+      </c>
+      <c r="B20" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" t="s">
+        <v>64</v>
+      </c>
+      <c r="D20" t="s">
+        <v>13</v>
+      </c>
+      <c r="E20" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>66</v>
+      </c>
+      <c r="B21" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" t="s">
+        <v>67</v>
+      </c>
+      <c r="D21" t="s">
+        <v>13</v>
+      </c>
+      <c r="E21" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>69</v>
+      </c>
+      <c r="B22" t="s">
+        <v>11</v>
+      </c>
+      <c r="C22" t="s">
+        <v>70</v>
+      </c>
+      <c r="D22" t="s">
+        <v>13</v>
+      </c>
+      <c r="E22" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>72</v>
+      </c>
+      <c r="B23" t="s">
+        <v>16</v>
+      </c>
+      <c r="C23" t="s">
+        <v>73</v>
+      </c>
+      <c r="D23" t="s">
+        <v>13</v>
+      </c>
+      <c r="E23" t="s">
+        <v>74</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Commiting with Configuration Definition
</commit_message>
<xml_diff>
--- a/src/test/resources/Sheet/Configsheet.xlsx
+++ b/src/test/resources/Sheet/Configsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jones\eclipse-workspace\Automation-QaPlateron\src\test\resources\Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{509CF12C-ED98-485F-9C47-4F52F13F8321}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D10C3FB-AEBE-40E4-97B3-0E610D864270}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="23280" windowHeight="12480" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="23280" windowHeight="12480" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -664,10 +664,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09244190-151A-43A4-A916-8BD3607753C8}">
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -676,125 +676,173 @@
     <col min="2" max="2" width="15.7109375" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="3" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>75</v>
       </c>
       <c r="B2" s="4">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>76</v>
       </c>
       <c r="B3" s="4"/>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>77</v>
       </c>
       <c r="B4" s="4"/>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>78</v>
       </c>
       <c r="B5" s="4"/>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>79</v>
       </c>
       <c r="B6" s="4"/>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>80</v>
       </c>
       <c r="B7" s="4"/>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>81</v>
       </c>
       <c r="B8" s="4"/>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>82</v>
       </c>
       <c r="B9" s="4">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>83</v>
       </c>
       <c r="B10" s="4">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>84</v>
       </c>
       <c r="B11" s="4">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>85</v>
       </c>
       <c r="B12" s="4">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>86</v>
       </c>
       <c r="B13" s="4">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>87</v>
       </c>
       <c r="B14" s="4">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>88</v>
       </c>
       <c r="B15" s="4">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>89</v>
       </c>
       <c r="B16" s="4">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>90</v>
       </c>
       <c r="B17" s="4">
+        <v>16</v>
+      </c>
+      <c r="C17">
         <v>16</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Completed Base changes for Checkbox
</commit_message>
<xml_diff>
--- a/src/test/resources/Sheet/Configsheet.xlsx
+++ b/src/test/resources/Sheet/Configsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jones\eclipse-workspace\Automation-QaPlateron\src\test\resources\Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D10C3FB-AEBE-40E4-97B3-0E610D864270}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9E64ED4-E490-458C-8E59-9F5DA656E3D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="23280" windowHeight="12480" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="23280" windowHeight="12480" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="96">
   <si>
     <t>Employee Name</t>
   </si>
@@ -254,24 +254,15 @@
     <t>+1 (923) 445 - 7210</t>
   </si>
   <si>
-    <t>Sales Tax</t>
-  </si>
-  <si>
     <t>Apply sales tax on the subtotal after deductions</t>
   </si>
   <si>
     <t>Apply sales tax on the tip after deductions</t>
   </si>
   <si>
-    <t>Service Fee Percentage</t>
-  </si>
-  <si>
     <t>Service Fee Percentage inclusive of sales tax</t>
   </si>
   <si>
-    <t>Service Fee Tax Percentage</t>
-  </si>
-  <si>
     <t>Apply service fee on the subtotal after deductions</t>
   </si>
   <si>
@@ -281,18 +272,12 @@
     <t>Gratuity Based on (Guest Count / Order Amount)</t>
   </si>
   <si>
-    <t>Gratuity percentage</t>
-  </si>
-  <si>
     <t>Guest count reaches this No</t>
   </si>
   <si>
     <t>subtotal reaches this amount</t>
   </si>
   <si>
-    <t>Gratuity Tax percentage</t>
-  </si>
-  <si>
     <t>Apply Gratuity for TakeAway</t>
   </si>
   <si>
@@ -302,16 +287,58 @@
     <t>Apply gratuity on the subtotal after deductions</t>
   </si>
   <si>
-    <t>Value</t>
+    <t>ON</t>
+  </si>
+  <si>
+    <t>OFF</t>
+  </si>
+  <si>
+    <t>Guest Count</t>
+  </si>
+  <si>
+    <t>Values</t>
+  </si>
+  <si>
+    <t>Configuring Entity</t>
+  </si>
+  <si>
+    <t>Gratuity percentage (%)</t>
+  </si>
+  <si>
+    <t>Gratuity Tax percentage (%)</t>
+  </si>
+  <si>
+    <t>Service Fee Tax Percentage (%)</t>
+  </si>
+  <si>
+    <t>Service Fee Percentage (%)</t>
+  </si>
+  <si>
+    <t>Sales Tax (%)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="20"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -359,17 +386,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -664,190 +690,157 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09244190-151A-43A4-A916-8BD3607753C8}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView zoomScale="70" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="48.5703125" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" style="5" customWidth="1"/>
+    <col min="1" max="1" width="82" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.28515625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1"/>
-      <c r="B1" s="3" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>75</v>
+    <row r="1" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A1" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A2" s="3" t="s">
+        <v>95</v>
       </c>
       <c r="B2" s="4">
         <v>10</v>
       </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+    </row>
+    <row r="3" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A3" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A4" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="C3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="B4" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A5" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B5" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A6" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B4" s="4"/>
-      <c r="C4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="B6" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A7" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B7" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A8" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="B5" s="4"/>
-      <c r="C5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="B8" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A9" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="B6" s="4"/>
-      <c r="C6">
+      <c r="B9" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A10" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A11" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B11" s="4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A12" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B12" s="4">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="B7" s="4"/>
-      <c r="C7">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="B8" s="4"/>
-      <c r="C8">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+    <row r="13" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A13" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="B9" s="4">
-        <v>8</v>
-      </c>
-      <c r="C9">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="B13" s="4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A14" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B14" s="4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A15" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="B10" s="4">
-        <v>9</v>
-      </c>
-      <c r="C10">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+      <c r="B15" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A16" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="B11" s="4">
-        <v>10</v>
-      </c>
-      <c r="C11">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+      <c r="B16" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A17" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="B12" s="4">
-        <v>11</v>
-      </c>
-      <c r="C12">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="B13" s="4">
-        <v>12</v>
-      </c>
-      <c r="C13">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+      <c r="B17" s="4" t="s">
         <v>87</v>
-      </c>
-      <c r="B14" s="4">
-        <v>13</v>
-      </c>
-      <c r="C14">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="B15" s="4">
-        <v>14</v>
-      </c>
-      <c r="C15">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="B16" s="4">
-        <v>15</v>
-      </c>
-      <c r="C16">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="B17" s="4">
-        <v>16</v>
-      </c>
-      <c r="C17">
-        <v>16</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -855,9 +848,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">

</xml_diff>

<commit_message>
Feature Completion Part -1 18: 20
</commit_message>
<xml_diff>
--- a/src/test/resources/Sheet/Configsheet.xlsx
+++ b/src/test/resources/Sheet/Configsheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jones\eclipse-workspace\Automation-QaPlateron\src\test\resources\Sheet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jones\eclipse-workspace\Automation-QAPlateron\src\test\resources\Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9E64ED4-E490-458C-8E59-9F5DA656E3D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92F836A8-0B84-4299-B80B-C2533D13F3C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="23280" windowHeight="12480" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="23280" windowHeight="12480" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -692,8 +692,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09244190-151A-43A4-A916-8BD3607753C8}">
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView zoomScale="70" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" zoomScale="70" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -835,7 +835,7 @@
         <v>85</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -848,7 +848,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Final Update on Bill Configuration -2
</commit_message>
<xml_diff>
--- a/src/test/resources/Sheet/Configsheet.xlsx
+++ b/src/test/resources/Sheet/Configsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jones\eclipse-workspace\Automation-QAPlateron\src\test\resources\Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92F836A8-0B84-4299-B80B-C2533D13F3C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1051F446-63C0-44E7-85BF-EE008EFE43EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="23280" windowHeight="12480" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -293,9 +293,6 @@
     <t>OFF</t>
   </si>
   <si>
-    <t>Guest Count</t>
-  </si>
-  <si>
     <t>Values</t>
   </si>
   <si>
@@ -315,6 +312,9 @@
   </si>
   <si>
     <t>Sales Tax (%)</t>
+  </si>
+  <si>
+    <t>Order Amount</t>
   </si>
 </sst>
 </file>
@@ -682,7 +682,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -693,40 +693,40 @@
   <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="82" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="24.33203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:2" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A1" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A2" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B2" s="4">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
+        <v>66.66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A3" s="3" t="s">
         <v>75</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A4" s="3" t="s">
         <v>76</v>
       </c>
@@ -734,87 +734,87 @@
         <v>86</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:2" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A5" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B5" s="4">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
+        <v>33.33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A6" s="3" t="s">
         <v>77</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A7" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B7" s="4">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
+        <v>19.63</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A8" s="3" t="s">
         <v>78</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A9" s="3" t="s">
         <v>79</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A10" s="3" t="s">
         <v>80</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A11" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B11" s="4">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
+        <v>75.989999999999995</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A12" s="3" t="s">
         <v>81</v>
       </c>
       <c r="B12" s="4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A13" s="3" t="s">
         <v>82</v>
       </c>
       <c r="B13" s="4">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A14" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B14" s="4">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A15" s="3" t="s">
         <v>83</v>
       </c>
@@ -822,20 +822,20 @@
         <v>86</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:2" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A16" s="3" t="s">
         <v>84</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A17" s="3" t="s">
         <v>85</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -852,16 +852,16 @@
       <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -878,7 +878,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -895,7 +895,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -912,7 +912,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -929,7 +929,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -946,7 +946,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -963,7 +963,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>25</v>
       </c>
@@ -980,7 +980,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>28</v>
       </c>
@@ -997,7 +997,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>28</v>
       </c>
@@ -1014,7 +1014,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -1031,7 +1031,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>36</v>
       </c>
@@ -1048,7 +1048,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>39</v>
       </c>
@@ -1065,7 +1065,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>42</v>
       </c>
@@ -1082,7 +1082,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>45</v>
       </c>
@@ -1099,7 +1099,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>48</v>
       </c>
@@ -1116,7 +1116,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>51</v>
       </c>
@@ -1133,7 +1133,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>54</v>
       </c>
@@ -1150,7 +1150,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>57</v>
       </c>
@@ -1167,7 +1167,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>60</v>
       </c>
@@ -1184,7 +1184,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>63</v>
       </c>
@@ -1201,7 +1201,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>66</v>
       </c>
@@ -1218,7 +1218,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>69</v>
       </c>
@@ -1235,7 +1235,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>72</v>
       </c>

</xml_diff>

<commit_message>
Cooking Station Feature Completion
</commit_message>
<xml_diff>
--- a/src/test/resources/Sheet/Configsheet.xlsx
+++ b/src/test/resources/Sheet/Configsheet.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1278" uniqueCount="343">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1408" uniqueCount="369">
   <si>
     <t>Employee Name</t>
   </si>
@@ -1059,6 +1059,84 @@
   </si>
   <si>
     <t>XRx8dmacYs</t>
+  </si>
+  <si>
+    <t>5050</t>
+  </si>
+  <si>
+    <t>+1 (154) 779 - 3376</t>
+  </si>
+  <si>
+    <t>4299</t>
+  </si>
+  <si>
+    <t>+1 (175) 550 - 7279</t>
+  </si>
+  <si>
+    <t>5520</t>
+  </si>
+  <si>
+    <t>+1 (158) 211 - 7544</t>
+  </si>
+  <si>
+    <t>9039</t>
+  </si>
+  <si>
+    <t>+1 (110) 546 - 0828</t>
+  </si>
+  <si>
+    <t>8631</t>
+  </si>
+  <si>
+    <t>+1 (104) 293 - 8995</t>
+  </si>
+  <si>
+    <t>8878</t>
+  </si>
+  <si>
+    <t>+1 (135) 241 - 8609</t>
+  </si>
+  <si>
+    <t>6228</t>
+  </si>
+  <si>
+    <t>+1 (120) 551 - 3724</t>
+  </si>
+  <si>
+    <t>5840</t>
+  </si>
+  <si>
+    <t>+1 (119) 309 - 7703</t>
+  </si>
+  <si>
+    <t>9741</t>
+  </si>
+  <si>
+    <t>+1 (175) 580 - 4060</t>
+  </si>
+  <si>
+    <t>1628</t>
+  </si>
+  <si>
+    <t>+1 (159) 332 - 3753</t>
+  </si>
+  <si>
+    <t>rKBHfhwLNL</t>
+  </si>
+  <si>
+    <t>7480</t>
+  </si>
+  <si>
+    <t>+1 (525) 657 - 7746</t>
+  </si>
+  <si>
+    <t>XqPKU2r66U</t>
+  </si>
+  <si>
+    <t>8220</t>
+  </si>
+  <si>
+    <t>+1 (239) 674 - 3948</t>
   </si>
 </sst>
 </file>
@@ -1654,172 +1732,172 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>194</v>
       </c>
       <c r="B3" t="s">
         <v>29</v>
       </c>
       <c r="C3" t="s">
-        <v>154</v>
+        <v>195</v>
       </c>
       <c r="D3" t="s">
         <v>13</v>
       </c>
       <c r="E3" t="s">
-        <v>155</v>
+        <v>196</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>171</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>246</v>
+        <v>343</v>
       </c>
       <c r="D4" t="s">
         <v>13</v>
       </c>
       <c r="E4" t="s">
-        <v>247</v>
+        <v>344</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>171</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>332</v>
+        <v>345</v>
       </c>
       <c r="D5" t="s">
         <v>13</v>
       </c>
       <c r="E5" t="s">
-        <v>333</v>
+        <v>346</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>156</v>
+        <v>171</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>157</v>
+        <v>347</v>
       </c>
       <c r="D6" t="s">
         <v>13</v>
       </c>
       <c r="E6" t="s">
-        <v>158</v>
+        <v>348</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>248</v>
+        <v>171</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>249</v>
+        <v>349</v>
       </c>
       <c r="D7" t="s">
         <v>13</v>
       </c>
       <c r="E7" t="s">
-        <v>250</v>
+        <v>350</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>159</v>
+        <v>171</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>160</v>
+        <v>351</v>
       </c>
       <c r="D8" t="s">
         <v>13</v>
       </c>
       <c r="E8" t="s">
-        <v>161</v>
+        <v>352</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>162</v>
+        <v>171</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="C9" t="s">
-        <v>163</v>
+        <v>353</v>
       </c>
       <c r="D9" t="s">
         <v>13</v>
       </c>
       <c r="E9" t="s">
-        <v>164</v>
+        <v>354</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>165</v>
+        <v>171</v>
       </c>
       <c r="B10" t="s">
         <v>11</v>
       </c>
       <c r="C10" t="s">
-        <v>166</v>
+        <v>355</v>
       </c>
       <c r="D10" t="s">
         <v>13</v>
       </c>
       <c r="E10" t="s">
-        <v>167</v>
+        <v>356</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>251</v>
+        <v>171</v>
       </c>
       <c r="B11" t="s">
         <v>11</v>
       </c>
       <c r="C11" t="s">
-        <v>252</v>
+        <v>357</v>
       </c>
       <c r="D11" t="s">
         <v>13</v>
       </c>
       <c r="E11" t="s">
-        <v>253</v>
+        <v>358</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="B12" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>169</v>
+        <v>359</v>
       </c>
       <c r="D12" t="s">
         <v>13</v>
       </c>
       <c r="E12" t="s">
-        <v>170</v>
+        <v>360</v>
       </c>
     </row>
     <row r="13">
@@ -1827,186 +1905,186 @@
         <v>171</v>
       </c>
       <c r="B13" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>172</v>
+        <v>361</v>
       </c>
       <c r="D13" t="s">
         <v>13</v>
       </c>
       <c r="E13" t="s">
-        <v>173</v>
+        <v>362</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>171</v>
+        <v>363</v>
       </c>
       <c r="B14" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="C14" t="s">
-        <v>174</v>
+        <v>364</v>
       </c>
       <c r="D14" t="s">
         <v>13</v>
       </c>
       <c r="E14" t="s">
-        <v>175</v>
+        <v>365</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>171</v>
+        <v>182</v>
       </c>
       <c r="B15" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="C15" t="s">
-        <v>176</v>
+        <v>183</v>
       </c>
       <c r="D15" t="s">
         <v>13</v>
       </c>
       <c r="E15" t="s">
-        <v>177</v>
+        <v>184</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>171</v>
+        <v>185</v>
       </c>
       <c r="B16" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="C16" t="s">
-        <v>178</v>
+        <v>186</v>
       </c>
       <c r="D16" t="s">
         <v>13</v>
       </c>
       <c r="E16" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>171</v>
+        <v>334</v>
       </c>
       <c r="B17" t="s">
         <v>11</v>
       </c>
       <c r="C17" t="s">
-        <v>180</v>
+        <v>335</v>
       </c>
       <c r="D17" t="s">
         <v>13</v>
       </c>
       <c r="E17" t="s">
-        <v>181</v>
+        <v>336</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="B18" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="C18" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="D18" t="s">
         <v>13</v>
       </c>
       <c r="E18" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>185</v>
+        <v>254</v>
       </c>
       <c r="B19" t="s">
         <v>29</v>
       </c>
       <c r="C19" t="s">
-        <v>186</v>
+        <v>255</v>
       </c>
       <c r="D19" t="s">
         <v>13</v>
       </c>
       <c r="E19" t="s">
-        <v>187</v>
+        <v>256</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>334</v>
+        <v>191</v>
       </c>
       <c r="B20" t="s">
         <v>11</v>
       </c>
       <c r="C20" t="s">
-        <v>335</v>
+        <v>192</v>
       </c>
       <c r="D20" t="s">
         <v>13</v>
       </c>
       <c r="E20" t="s">
-        <v>336</v>
+        <v>193</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>188</v>
+        <v>366</v>
       </c>
       <c r="B21" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="C21" t="s">
-        <v>189</v>
+        <v>367</v>
       </c>
       <c r="D21" t="s">
         <v>13</v>
       </c>
       <c r="E21" t="s">
-        <v>190</v>
+        <v>368</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>254</v>
+        <v>337</v>
       </c>
       <c r="B22" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="C22" t="s">
-        <v>255</v>
+        <v>338</v>
       </c>
       <c r="D22" t="s">
         <v>13</v>
       </c>
       <c r="E22" t="s">
-        <v>256</v>
+        <v>339</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="B23" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="C23" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="D23" t="s">
         <v>13</v>
       </c>
       <c r="E23" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
     </row>
     <row r="24">

</xml_diff>

<commit_message>
Order Completion part 2
</commit_message>
<xml_diff>
--- a/src/test/resources/Sheet/Configsheet.xlsx
+++ b/src/test/resources/Sheet/Configsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jones\eclipse-workspace\Automation-QAPlateron\src\test\resources\Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{750D0FCA-9C72-4993-A99E-FC8131783CC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1F057F7-8414-47C7-9FBD-0336CA53370F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill Configuration" sheetId="3" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="579" uniqueCount="289">
   <si>
     <t>Employee Name</t>
   </si>
@@ -915,6 +915,9 @@
   </si>
   <si>
     <t>Automation Area</t>
+  </si>
+  <si>
+    <t>Auto 7</t>
   </si>
 </sst>
 </file>
@@ -1355,8 +1358,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09244190-151A-43A4-A916-8BD3607753C8}">
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView zoomScale="70" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+    <sheetView tabSelected="1" zoomScale="70" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1498,7 +1501,7 @@
         <v>58</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -3371,10 +3374,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA6CF15C-C633-4176-8909-CF9532871AF5}">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3422,13 +3425,13 @@
         <v>10</v>
       </c>
       <c r="C2" s="7">
-        <v>99</v>
+        <v>10</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>156</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="F2" s="7" t="s">
         <v>156</v>
@@ -3445,16 +3448,16 @@
         <v>172</v>
       </c>
       <c r="B3" s="7">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="C3" s="7">
-        <v>49</v>
+        <v>25</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>156</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="F3" s="7" t="s">
         <v>157</v>
@@ -3468,22 +3471,22 @@
         <v>173</v>
       </c>
       <c r="B4" s="7">
-        <v>15</v>
+        <v>23.33</v>
       </c>
       <c r="C4" s="7">
-        <v>51</v>
+        <v>1</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F4" s="7" t="s">
         <v>157</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -3491,19 +3494,19 @@
         <v>174</v>
       </c>
       <c r="B5" s="7">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="C5" s="7">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>156</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="G5" s="7" t="s">
         <v>157</v>
@@ -3514,16 +3517,16 @@
         <v>175</v>
       </c>
       <c r="B6" s="7">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="C6" s="7">
-        <v>0</v>
+        <v>199</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="F6" s="7" t="s">
         <v>156</v>
@@ -3537,7 +3540,7 @@
         <v>176</v>
       </c>
       <c r="B7" s="7">
-        <v>50</v>
+        <v>28</v>
       </c>
       <c r="C7" s="7">
         <v>70</v>
@@ -3549,13 +3552,37 @@
         <v>156</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G7" s="7" t="s">
         <v>157</v>
       </c>
     </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>288</v>
+      </c>
+      <c r="B8" s="7">
+        <v>66.66</v>
+      </c>
+      <c r="C8" s="7">
+        <v>160</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>157</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Pos Table Management almost finished
</commit_message>
<xml_diff>
--- a/src/test/resources/Sheet/Configsheet.xlsx
+++ b/src/test/resources/Sheet/Configsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\booba\eclipse-workspace\Automation-QAPlateron\src\test\resources\Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AD3BF98-88CE-48D5-992C-5F9B72841FF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74C8EAAF-9AF5-4198-89CF-FF2895D133E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill Configuration" sheetId="3" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="237">
   <si>
     <t>Employee Name</t>
   </si>
@@ -713,21 +713,9 @@
     <t>S3</t>
   </si>
   <si>
-    <t>33</t>
-  </si>
-  <si>
-    <t>S2</t>
-  </si>
-  <si>
-    <t>22</t>
-  </si>
-  <si>
     <t>xyz</t>
   </si>
   <si>
-    <t>77</t>
-  </si>
-  <si>
     <t>S1</t>
   </si>
   <si>
@@ -749,10 +737,31 @@
     <t>T7</t>
   </si>
   <si>
-    <t>47</t>
-  </si>
-  <si>
     <t>AutoEdited</t>
+  </si>
+  <si>
+    <t>G1</t>
+  </si>
+  <si>
+    <t>S4</t>
+  </si>
+  <si>
+    <t>T4</t>
+  </si>
+  <si>
+    <t>T5</t>
+  </si>
+  <si>
+    <t>T6</t>
+  </si>
+  <si>
+    <t>T8</t>
+  </si>
+  <si>
+    <t>T9</t>
+  </si>
+  <si>
+    <t>T10</t>
   </si>
 </sst>
 </file>
@@ -878,7 +887,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -911,6 +920,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2732,10 +2744,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{903D10E7-7786-40C4-B45B-1A0F5269C7C8}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2767,10 +2779,10 @@
         <v>218</v>
       </c>
       <c r="B3" t="s">
-        <v>219</v>
-      </c>
-      <c r="C3" t="s">
-        <v>220</v>
+        <v>229</v>
+      </c>
+      <c r="C3" s="16">
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -2780,8 +2792,8 @@
       <c r="B4" t="s">
         <v>221</v>
       </c>
-      <c r="C4" t="s">
-        <v>222</v>
+      <c r="C4" s="16">
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -2789,10 +2801,10 @@
         <v>218</v>
       </c>
       <c r="B5" t="s">
-        <v>223</v>
-      </c>
-      <c r="C5" t="s">
-        <v>224</v>
+        <v>219</v>
+      </c>
+      <c r="C5" s="16">
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -2800,46 +2812,157 @@
         <v>218</v>
       </c>
       <c r="B6" t="s">
-        <v>225</v>
-      </c>
-      <c r="C6" t="s">
-        <v>217</v>
+        <v>230</v>
+      </c>
+      <c r="C6" s="16">
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
       <c r="B7" t="s">
-        <v>227</v>
-      </c>
-      <c r="C7" t="s">
-        <v>113</v>
+        <v>220</v>
+      </c>
+      <c r="C7" s="16">
+        <v>77</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="B8" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="C8" t="s">
-        <v>230</v>
+        <v>113</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>224</v>
+      </c>
+      <c r="B9" t="s">
+        <v>225</v>
+      </c>
+      <c r="C9" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>228</v>
+      </c>
+      <c r="B10" t="s">
+        <v>216</v>
+      </c>
+      <c r="C10" s="16">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>228</v>
+      </c>
+      <c r="B11" t="s">
+        <v>223</v>
+      </c>
+      <c r="C11" s="16">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>228</v>
+      </c>
+      <c r="B12" t="s">
+        <v>225</v>
+      </c>
+      <c r="C12" s="16">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>228</v>
+      </c>
+      <c r="B13" t="s">
+        <v>231</v>
+      </c>
+      <c r="C13" s="16">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>228</v>
+      </c>
+      <c r="B14" t="s">
+        <v>232</v>
+      </c>
+      <c r="C14" s="16">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>228</v>
+      </c>
+      <c r="B15" t="s">
         <v>233</v>
       </c>
-      <c r="B9" t="s">
-        <v>231</v>
-      </c>
-      <c r="C9" t="s">
-        <v>232</v>
+      <c r="C15" s="16">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>228</v>
+      </c>
+      <c r="B16" t="s">
+        <v>227</v>
+      </c>
+      <c r="C16" s="16">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>228</v>
+      </c>
+      <c r="B17" t="s">
+        <v>234</v>
+      </c>
+      <c r="C17" s="16">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>228</v>
+      </c>
+      <c r="B18" t="s">
+        <v>235</v>
+      </c>
+      <c r="C18" s="16">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>228</v>
+      </c>
+      <c r="B19" t="s">
+        <v>236</v>
+      </c>
+      <c r="C19" s="16">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Decline Flow Feature File and Step Update
</commit_message>
<xml_diff>
--- a/src/test/resources/Sheet/Configsheet.xlsx
+++ b/src/test/resources/Sheet/Configsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jones\eclipse-workspace\Automation-QAPlateron\src\test\resources\Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{376CA1E3-733F-4ED6-8513-74983C453268}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DA62E4B-376D-4AA0-A1B4-BEDE1B7A1FAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill Configuration" sheetId="3" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="197">
   <si>
     <t>PhoneNo</t>
   </si>
@@ -549,9 +549,6 @@
     <t>Menu Item18</t>
   </si>
   <si>
-    <t>0.99</t>
-  </si>
-  <si>
     <t>Menu Item19</t>
   </si>
   <si>
@@ -573,22 +570,10 @@
     <t>7.99</t>
   </si>
   <si>
-    <t>qXaqzFcH4h</t>
-  </si>
-  <si>
-    <t>RCkVPcscIl</t>
-  </si>
-  <si>
-    <t>cLLWQ7g0De</t>
-  </si>
-  <si>
     <t>Required</t>
   </si>
   <si>
     <t>Optional</t>
-  </si>
-  <si>
-    <t>Both</t>
   </si>
   <si>
     <t>Nil</t>
@@ -722,12 +707,45 @@
       <t>(Guest Count / Order Amount)</t>
     </r>
   </si>
+  <si>
+    <t>KfftCvg3df</t>
+  </si>
+  <si>
+    <t>ZzCTLnaaTj</t>
+  </si>
+  <si>
+    <t>0.00</t>
+  </si>
+  <si>
+    <t>J2T4ZcI811</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>Mod 1</t>
+  </si>
+  <si>
+    <t>Mod 2</t>
+  </si>
+  <si>
+    <t>Mod 3</t>
+  </si>
+  <si>
+    <t>Max</t>
+  </si>
+  <si>
+    <t>Min</t>
+  </si>
+  <si>
+    <t>Required and Optional</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -775,8 +793,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -801,8 +826,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -862,11 +899,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -904,11 +954,29 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1192,7 +1260,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09244190-151A-43A4-A916-8BD3607753C8}">
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" workbookViewId="0">
+    <sheetView zoomScale="70" workbookViewId="0">
       <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
@@ -1227,7 +1295,7 @@
         <v>6</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
@@ -1238,7 +1306,7 @@
         <v>5</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
@@ -1251,7 +1319,7 @@
     </row>
     <row r="6" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A6" s="3" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="B6" s="18" t="s">
         <v>5</v>
@@ -1267,7 +1335,7 @@
     </row>
     <row r="8" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A8" s="3" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="B8" s="18" t="s">
         <v>5</v>
@@ -1275,7 +1343,7 @@
     </row>
     <row r="9" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A9" s="3" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="B9" s="18" t="s">
         <v>5</v>
@@ -1283,7 +1351,7 @@
     </row>
     <row r="10" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A10" s="3" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="B10" s="18" t="s">
         <v>13</v>
@@ -1315,7 +1383,7 @@
     </row>
     <row r="14" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A14" s="3" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="B14" s="18">
         <v>51</v>
@@ -1323,27 +1391,27 @@
     </row>
     <row r="15" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A15" s="3" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="B15" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="C15" s="19" t="s">
-        <v>180</v>
+      <c r="C15" s="24" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A16" s="3" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="B16" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="C16" s="20"/>
+      <c r="C16" s="25"/>
     </row>
     <row r="17" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A17" s="3" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="B17" s="18" t="s">
         <v>5</v>
@@ -1351,10 +1419,10 @@
     </row>
     <row r="18" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A18" s="17" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="B18" s="18" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
     </row>
   </sheetData>
@@ -1492,10 +1560,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A4B9F6E-5FE6-4DB9-9728-EB3DF1F23798}">
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1504,356 +1572,438 @@
     <col min="2" max="2" width="24.28515625" style="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="21" style="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="22.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15" customWidth="1"/>
+    <col min="5" max="5" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.28515625" customWidth="1"/>
+    <col min="7" max="7" width="16" customWidth="1"/>
+    <col min="9" max="9" width="12.42578125" customWidth="1"/>
+    <col min="11" max="11" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="8" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="22" t="s">
+        <v>186</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="22" t="s">
+        <v>186</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="22" t="s">
+        <v>186</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="22" t="s">
+        <v>186</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="22" t="s">
+        <v>186</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="22" t="s">
+        <v>186</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="22" t="s">
+        <v>186</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="22" t="s">
+        <v>186</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="22" t="s">
+        <v>186</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="22" t="s">
+        <v>186</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="22" t="s">
+        <v>187</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="22" t="s">
+        <v>187</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="22" t="s">
+        <v>187</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="22" t="s">
+        <v>187</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="22" t="s">
+        <v>187</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="22" t="s">
+        <v>187</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="22" t="s">
+        <v>187</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="22" t="s">
+        <v>187</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>188</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="22" t="s">
+        <v>187</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="F20" s="26" t="s">
+        <v>191</v>
+      </c>
+      <c r="G20" s="26"/>
+      <c r="H20" s="26" t="s">
+        <v>192</v>
+      </c>
+      <c r="I20" s="26"/>
+      <c r="J20" s="26" t="s">
+        <v>193</v>
+      </c>
+      <c r="K20" s="26"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="22" t="s">
+        <v>187</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="F21" s="19" t="s">
+        <v>195</v>
+      </c>
+      <c r="G21" s="19" t="s">
+        <v>194</v>
+      </c>
+      <c r="H21" s="19" t="s">
+        <v>195</v>
+      </c>
+      <c r="I21" s="19" t="s">
+        <v>194</v>
+      </c>
+      <c r="J21" s="19" t="s">
+        <v>195</v>
+      </c>
+      <c r="K21" s="19" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="22" t="s">
+        <v>189</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="E22" s="21" t="s">
+        <v>172</v>
+      </c>
+      <c r="F22" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="G22" s="23" t="s">
+        <v>190</v>
+      </c>
+      <c r="H22" s="20"/>
+      <c r="I22" s="20"/>
+      <c r="J22" s="20"/>
+      <c r="K22" s="20"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="22" t="s">
+        <v>189</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="E23" s="21" t="s">
+        <v>196</v>
+      </c>
+      <c r="F23" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="G23" s="23" t="s">
+        <v>190</v>
+      </c>
+      <c r="H23" s="20" t="s">
+        <v>108</v>
+      </c>
+      <c r="I23" s="20" t="s">
+        <v>190</v>
+      </c>
+      <c r="J23" s="20"/>
+      <c r="K23" s="20"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="22" t="s">
+        <v>189</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="E24" s="21" t="s">
         <v>173</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
-        <v>174</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
-        <v>174</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="C13" s="1" t="s">
+      <c r="F24" s="20" t="s">
         <v>108</v>
       </c>
-      <c r="D13" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
-        <v>174</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
-        <v>174</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
-        <v>174</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
-        <v>174</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
-        <v>174</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
-        <v>174</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
-        <v>174</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
-        <v>174</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="5" t="s">
-        <v>175</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
-        <v>175</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="5" t="s">
-        <v>175</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>177</v>
+      <c r="G24" s="20" t="s">
+        <v>190</v>
+      </c>
+      <c r="H24" s="20" t="s">
+        <v>108</v>
+      </c>
+      <c r="I24" s="20" t="s">
+        <v>190</v>
+      </c>
+      <c r="J24" s="20" t="s">
+        <v>108</v>
+      </c>
+      <c r="K24" s="20" t="s">
+        <v>190</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="J20:K20"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1861,7 +2011,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Step Definition Update part -1
</commit_message>
<xml_diff>
--- a/src/test/resources/Sheet/Configsheet.xlsx
+++ b/src/test/resources/Sheet/Configsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jones\eclipse-workspace\Automation-QAPlateron\src\test\resources\Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DA62E4B-376D-4AA0-A1B4-BEDE1B7A1FAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA5C38A9-3F9E-4C26-8C4E-15B526780FAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill Configuration" sheetId="3" r:id="rId1"/>
@@ -717,9 +717,6 @@
     <t>0.00</t>
   </si>
   <si>
-    <t>J2T4ZcI811</t>
-  </si>
-  <si>
     <t>4</t>
   </si>
   <si>
@@ -739,6 +736,9 @@
   </si>
   <si>
     <t>Required and Optional</t>
+  </si>
+  <si>
+    <t>pFiMb9HUdJ</t>
   </si>
 </sst>
 </file>
@@ -916,7 +916,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -965,9 +965,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1396,7 +1393,7 @@
       <c r="B15" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="C15" s="24" t="s">
+      <c r="C15" s="23" t="s">
         <v>175</v>
       </c>
     </row>
@@ -1407,7 +1404,7 @@
       <c r="B16" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="C16" s="25"/>
+      <c r="C16" s="24"/>
     </row>
     <row r="17" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A17" s="3" t="s">
@@ -1562,8 +1559,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A4B9F6E-5FE6-4DB9-9728-EB3DF1F23798}">
   <dimension ref="A1:K24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1858,18 +1855,18 @@
       <c r="D20" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="F20" s="26" t="s">
+      <c r="F20" s="25" t="s">
+        <v>190</v>
+      </c>
+      <c r="G20" s="25"/>
+      <c r="H20" s="25" t="s">
         <v>191</v>
       </c>
-      <c r="G20" s="26"/>
-      <c r="H20" s="26" t="s">
+      <c r="I20" s="25"/>
+      <c r="J20" s="25" t="s">
         <v>192</v>
       </c>
-      <c r="I20" s="26"/>
-      <c r="J20" s="26" t="s">
-        <v>193</v>
-      </c>
-      <c r="K20" s="26"/>
+      <c r="K20" s="25"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="22" t="s">
@@ -1885,45 +1882,45 @@
         <v>136</v>
       </c>
       <c r="F21" s="19" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G21" s="19" t="s">
+        <v>193</v>
+      </c>
+      <c r="H21" s="19" t="s">
         <v>194</v>
       </c>
-      <c r="H21" s="19" t="s">
-        <v>195</v>
-      </c>
       <c r="I21" s="19" t="s">
+        <v>193</v>
+      </c>
+      <c r="J21" s="19" t="s">
         <v>194</v>
       </c>
-      <c r="J21" s="19" t="s">
-        <v>195</v>
-      </c>
       <c r="K21" s="19" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="22" t="s">
-        <v>189</v>
-      </c>
-      <c r="B22" s="8" t="s">
+      <c r="A22" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="C22" s="8" t="s">
+      <c r="C22" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="D22" s="8" t="s">
+      <c r="D22" s="1" t="s">
         <v>133</v>
       </c>
       <c r="E22" s="21" t="s">
         <v>172</v>
       </c>
-      <c r="F22" s="23" t="s">
+      <c r="F22" t="s">
         <v>108</v>
       </c>
-      <c r="G22" s="23" t="s">
-        <v>190</v>
+      <c r="G22" t="s">
+        <v>189</v>
       </c>
       <c r="H22" s="20"/>
       <c r="I22" s="20"/>
@@ -1931,69 +1928,69 @@
       <c r="K22" s="20"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="22" t="s">
-        <v>189</v>
-      </c>
-      <c r="B23" s="8" t="s">
+      <c r="A23" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="C23" s="8" t="s">
+      <c r="C23" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="D23" s="8" t="s">
+      <c r="D23" s="1" t="s">
         <v>130</v>
       </c>
       <c r="E23" s="21" t="s">
-        <v>196</v>
-      </c>
-      <c r="F23" s="23" t="s">
-        <v>108</v>
-      </c>
-      <c r="G23" s="23" t="s">
-        <v>190</v>
-      </c>
-      <c r="H23" s="20" t="s">
-        <v>108</v>
-      </c>
-      <c r="I23" s="20" t="s">
-        <v>190</v>
+        <v>195</v>
+      </c>
+      <c r="F23" t="s">
+        <v>110</v>
+      </c>
+      <c r="G23" t="s">
+        <v>110</v>
+      </c>
+      <c r="H23" t="s">
+        <v>110</v>
+      </c>
+      <c r="I23" t="s">
+        <v>110</v>
       </c>
       <c r="J23" s="20"/>
       <c r="K23" s="20"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="22" t="s">
-        <v>189</v>
-      </c>
-      <c r="B24" s="8" t="s">
+      <c r="A24" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="C24" s="8" t="s">
+      <c r="C24" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="D24" s="8" t="s">
+      <c r="D24" s="1" t="s">
         <v>136</v>
       </c>
       <c r="E24" s="21" t="s">
         <v>173</v>
       </c>
-      <c r="F24" s="20" t="s">
+      <c r="F24" t="s">
         <v>108</v>
       </c>
-      <c r="G24" s="20" t="s">
-        <v>190</v>
-      </c>
-      <c r="H24" s="20" t="s">
+      <c r="G24" t="s">
+        <v>189</v>
+      </c>
+      <c r="H24" t="s">
         <v>108</v>
       </c>
-      <c r="I24" s="20" t="s">
-        <v>190</v>
-      </c>
-      <c r="J24" s="20" t="s">
+      <c r="I24" t="s">
+        <v>189</v>
+      </c>
+      <c r="J24" t="s">
         <v>108</v>
       </c>
-      <c r="K24" s="20" t="s">
-        <v>190</v>
+      <c r="K24" t="s">
+        <v>189</v>
       </c>
     </row>
   </sheetData>
@@ -2011,7 +2008,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Calculation Rewamp with Decline flow update
</commit_message>
<xml_diff>
--- a/src/test/resources/Sheet/Configsheet.xlsx
+++ b/src/test/resources/Sheet/Configsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jones\eclipse-workspace\Automation-QAPlateron\src\test\resources\Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA5C38A9-3F9E-4C26-8C4E-15B526780FAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{544F0027-605F-4AFF-9AED-B9CA78EBAF35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill Configuration" sheetId="3" r:id="rId1"/>
@@ -40,8 +40,42 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>jones</author>
+  </authors>
+  <commentList>
+    <comment ref="B7" authorId="0" shapeId="0" xr:uid="{E0EA99F3-94E2-417F-B1F0-54E9AFA13CAF}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="14"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>jones:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="14"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Service Fee Percentage</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="198">
   <si>
     <t>PhoneNo</t>
   </si>
@@ -740,12 +774,15 @@
   <si>
     <t>pFiMb9HUdJ</t>
   </si>
+  <si>
+    <t>Excluded Items</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -799,6 +836,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="7">
@@ -916,7 +966,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -974,6 +1024,9 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1254,11 +1307,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09244190-151A-43A4-A916-8BD3607753C8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09244190-151A-43A4-A916-8BD3607753C8}">
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView zoomScale="70" workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1327,7 +1380,7 @@
         <v>10</v>
       </c>
       <c r="B7" s="18">
-        <v>33.33</v>
+        <v>66.66</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
@@ -1428,6 +1481,7 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1559,7 +1613,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A4B9F6E-5FE6-4DB9-9728-EB3DF1F23798}">
   <dimension ref="A1:K24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
@@ -2751,10 +2805,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA6CF15C-C633-4176-8909-CF9532871AF5}">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2811,7 +2865,7 @@
         <v>35</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G2" s="7" t="s">
         <v>35</v>
@@ -2883,7 +2937,7 @@
         <v>36</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G5" s="7" t="s">
         <v>36</v>
@@ -2958,7 +3012,17 @@
         <v>36</v>
       </c>
     </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="26" t="s">
+        <v>197</v>
+      </c>
+      <c r="B10" s="26"/>
+      <c r="C10" s="26"/>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A10:C10"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Select Menu and Settings
</commit_message>
<xml_diff>
--- a/src/test/resources/Sheet/Configsheet.xlsx
+++ b/src/test/resources/Sheet/Configsheet.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jones\eclipse-workspace\Automation-QAPlateron\src\test\resources\Sheet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\booba\eclipse-workspace\Automation-QAPlateron\src\test\resources\Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{544F0027-605F-4AFF-9AED-B9CA78EBAF35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB4F2621-DB29-4523-88C9-6EC2BA732E00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="782" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill Configuration" sheetId="3" r:id="rId1"/>
@@ -24,7 +24,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -40,42 +40,8 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>jones</author>
-  </authors>
-  <commentList>
-    <comment ref="B7" authorId="0" shapeId="0" xr:uid="{E0EA99F3-94E2-417F-B1F0-54E9AFA13CAF}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="14"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>jones:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="14"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Service Fee Percentage</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="201">
   <si>
     <t>PhoneNo</t>
   </si>
@@ -775,14 +741,24 @@
     <t>pFiMb9HUdJ</t>
   </si>
   <si>
-    <t>Excluded Items</t>
+    <t>Cooking Stations Name</t>
+  </si>
+  <si>
+    <t>Station K6LN9zkLsa</t>
+  </si>
+  <si>
+    <t>Station mBZilaBX33</t>
+  </si>
+  <si>
+    <t>Station xQFyhOvNop</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -839,16 +815,11 @@
     </font>
     <font>
       <b/>
-      <sz val="14"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="7">
@@ -889,7 +860,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -962,11 +933,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1025,8 +1005,14 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1307,18 +1293,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09244190-151A-43A4-A916-8BD3607753C8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09244190-151A-43A4-A916-8BD3607753C8}">
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView zoomScale="70" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="102.140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="24.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="52.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="102.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="1" width="24.28515625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="52.85546875"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
@@ -1380,7 +1366,7 @@
         <v>10</v>
       </c>
       <c r="B7" s="18">
-        <v>66.66</v>
+        <v>33.33</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
@@ -1481,7 +1467,6 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1490,117 +1475,117 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10.85546875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="23.5703125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="32" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="15.7109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="10.85546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="23.5703125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="32.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>89</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>90</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" t="s" s="0">
         <v>91</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" t="s" s="0">
         <v>92</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" t="s" s="0">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>93</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>94</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>95</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" t="s" s="0">
         <v>96</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" t="s" s="0">
         <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>97</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>98</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="s" s="0">
         <v>99</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" t="s" s="0">
         <v>100</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" t="s" s="0">
         <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" t="s" s="0">
         <v>97</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" t="s" s="0">
         <v>98</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" t="s" s="0">
         <v>101</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" t="s" s="0">
         <v>100</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" t="s" s="0">
         <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" t="s" s="0">
         <v>102</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" t="s" s="0">
         <v>103</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" t="s" s="0">
         <v>104</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" t="s" s="0">
         <v>100</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" t="s" s="0">
         <v>87</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" t="s" s="0">
         <v>105</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" t="s" s="0">
         <v>106</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" t="s" s="0">
         <v>107</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" t="s" s="0">
         <v>100</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" t="s" s="0">
         <v>88</v>
       </c>
     </row>
@@ -1613,38 +1598,41 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A4B9F6E-5FE6-4DB9-9728-EB3DF1F23798}">
   <dimension ref="A1:K24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" style="5" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="24.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="21" style="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="22.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.28515625" customWidth="1"/>
-    <col min="7" max="7" width="16" customWidth="1"/>
-    <col min="9" max="9" width="12.42578125" customWidth="1"/>
-    <col min="11" max="11" width="11.140625" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" style="5" width="17.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="1" width="24.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="1" width="21.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="1" width="22.42578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="21.42578125"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="21.85546875"/>
+    <col min="7" max="7" customWidth="true" width="16.0"/>
+    <col min="9" max="9" customWidth="true" width="12.42578125"/>
+    <col min="11" max="11" customWidth="true" width="11.140625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="28" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F1" s="26" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
         <v>186</v>
       </c>
@@ -1657,8 +1645,11 @@
       <c r="D2" s="8" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F2" t="s" s="0">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="22" t="s">
         <v>186</v>
       </c>
@@ -1671,8 +1662,11 @@
       <c r="D3" s="8" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F3" t="s" s="0">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="22" t="s">
         <v>186</v>
       </c>
@@ -1685,8 +1679,11 @@
       <c r="D4" s="8" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F4" t="s" s="0">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="22" t="s">
         <v>186</v>
       </c>
@@ -1700,7 +1697,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="22" t="s">
         <v>186</v>
       </c>
@@ -1714,7 +1711,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="22" t="s">
         <v>186</v>
       </c>
@@ -1728,7 +1725,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="22" t="s">
         <v>186</v>
       </c>
@@ -1742,7 +1739,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="22" t="s">
         <v>186</v>
       </c>
@@ -1756,7 +1753,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="22" t="s">
         <v>186</v>
       </c>
@@ -1770,7 +1767,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="22" t="s">
         <v>186</v>
       </c>
@@ -1784,7 +1781,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="22" t="s">
         <v>187</v>
       </c>
@@ -1798,7 +1795,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="22" t="s">
         <v>187</v>
       </c>
@@ -1812,7 +1809,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="22" t="s">
         <v>187</v>
       </c>
@@ -1826,7 +1823,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="22" t="s">
         <v>187</v>
       </c>
@@ -1840,7 +1837,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="22" t="s">
         <v>187</v>
       </c>
@@ -1970,10 +1967,10 @@
       <c r="E22" s="21" t="s">
         <v>172</v>
       </c>
-      <c r="F22" t="s">
+      <c r="F22" t="s" s="0">
         <v>108</v>
       </c>
-      <c r="G22" t="s">
+      <c r="G22" t="s" s="0">
         <v>189</v>
       </c>
       <c r="H22" s="20"/>
@@ -1997,16 +1994,16 @@
       <c r="E23" s="21" t="s">
         <v>195</v>
       </c>
-      <c r="F23" t="s">
+      <c r="F23" t="s" s="0">
         <v>110</v>
       </c>
-      <c r="G23" t="s">
+      <c r="G23" t="s" s="0">
         <v>110</v>
       </c>
-      <c r="H23" t="s">
+      <c r="H23" t="s" s="0">
         <v>110</v>
       </c>
-      <c r="I23" t="s">
+      <c r="I23" t="s" s="0">
         <v>110</v>
       </c>
       <c r="J23" s="20"/>
@@ -2028,22 +2025,22 @@
       <c r="E24" s="21" t="s">
         <v>173</v>
       </c>
-      <c r="F24" t="s">
+      <c r="F24" t="s" s="0">
         <v>108</v>
       </c>
-      <c r="G24" t="s">
+      <c r="G24" t="s" s="0">
         <v>189</v>
       </c>
-      <c r="H24" t="s">
+      <c r="H24" t="s" s="0">
         <v>108</v>
       </c>
-      <c r="I24" t="s">
+      <c r="I24" t="s" s="0">
         <v>189</v>
       </c>
-      <c r="J24" t="s">
+      <c r="J24" t="s" s="0">
         <v>108</v>
       </c>
-      <c r="K24" t="s">
+      <c r="K24" t="s" s="0">
         <v>189</v>
       </c>
     </row>
@@ -2063,21 +2060,21 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H35" sqref="H35"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="21.140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="9.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="21.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="1" width="9.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>111</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>112</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -2085,10 +2082,10 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>113</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>114</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -2096,10 +2093,10 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>113</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>115</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -2107,10 +2104,10 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" t="s" s="0">
         <v>113</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" t="s" s="0">
         <v>116</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -2118,10 +2115,10 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" t="s" s="0">
         <v>113</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" t="s" s="0">
         <v>117</v>
       </c>
       <c r="C5" s="1" t="s">
@@ -2129,10 +2126,10 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" t="s" s="0">
         <v>118</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" t="s" s="0">
         <v>119</v>
       </c>
       <c r="C6" s="1" t="s">
@@ -2140,10 +2137,10 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" t="s" s="0">
         <v>118</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" t="s" s="0">
         <v>120</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -2151,10 +2148,10 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" t="s" s="0">
         <v>118</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" t="s" s="0">
         <v>121</v>
       </c>
       <c r="C8" s="1" t="s">
@@ -2162,10 +2159,10 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" t="s" s="0">
         <v>118</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" t="s" s="0">
         <v>122</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -2173,10 +2170,10 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" t="s" s="0">
         <v>123</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" t="s" s="0">
         <v>124</v>
       </c>
       <c r="C10" s="1" t="s">
@@ -2184,10 +2181,10 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" t="s" s="0">
         <v>123</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" t="s" s="0">
         <v>125</v>
       </c>
       <c r="C11" s="1" t="s">
@@ -2195,10 +2192,10 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="A12" t="s" s="0">
         <v>123</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" t="s" s="0">
         <v>126</v>
       </c>
       <c r="C12" s="1" t="s">
@@ -2206,10 +2203,10 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="A13" t="s" s="0">
         <v>123</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" t="s" s="0">
         <v>127</v>
       </c>
       <c r="C13" s="1" t="s">
@@ -2231,16 +2228,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="25.42578125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="20" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="18.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.140625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="19" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="11.85546875" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13.85546875" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.140625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="21.42578125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="25.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="20.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="18.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="17.140625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="11.85546875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -2678,18 +2675,18 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="21.42578125" style="1" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="19.0"/>
+    <col min="2" max="2" customWidth="true" style="1" width="11.7109375"/>
+    <col min="3" max="3" customWidth="true" style="1" width="21.42578125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>59</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -2700,7 +2697,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>62</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -2711,7 +2708,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>65</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -2722,7 +2719,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" t="s" s="0">
         <v>65</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -2733,7 +2730,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" t="s" s="0">
         <v>65</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -2744,7 +2741,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" t="s" s="0">
         <v>65</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -2755,7 +2752,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" t="s" s="0">
         <v>65</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -2766,7 +2763,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" t="s" s="0">
         <v>75</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -2777,7 +2774,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" t="s" s="0">
         <v>77</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -2788,7 +2785,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" t="s" s="0">
         <v>80</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -2805,21 +2802,21 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA6CF15C-C633-4176-8909-CF9532871AF5}">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="23.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="38.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="33" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="21.7109375" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="21.28515625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="23.28515625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="38.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="10.85546875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="33.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="21.7109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="21.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="14" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2865,7 +2862,7 @@
         <v>35</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G2" s="7" t="s">
         <v>35</v>
@@ -2937,7 +2934,7 @@
         <v>36</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G5" s="7" t="s">
         <v>36</v>
@@ -3012,17 +3009,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="26" t="s">
-        <v>197</v>
-      </c>
-      <c r="B10" s="26"/>
-      <c r="C10" s="26"/>
-    </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A10:C10"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Void All Items Flows Completion - 5
</commit_message>
<xml_diff>
--- a/src/test/resources/Sheet/Configsheet.xlsx
+++ b/src/test/resources/Sheet/Configsheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\booba\eclipse-workspace\Automation-QAPlateron\src\test\resources\Sheet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jones\eclipse-workspace\Automation-QAPlateron\src\test\resources\Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB4F2621-DB29-4523-88C9-6EC2BA732E00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1FCCA10-9EBD-413B-9697-2990ECAFBAD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="782" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="42420" yWindow="0" windowWidth="15180" windowHeight="14040" tabRatio="782" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill Configuration" sheetId="3" r:id="rId1"/>
@@ -24,7 +24,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -757,7 +757,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -996,6 +995,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1003,15 +1011,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1296,15 +1295,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09244190-151A-43A4-A916-8BD3607753C8}">
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView zoomScale="70" workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+    <sheetView tabSelected="1" zoomScale="70" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="102.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="1" width="24.28515625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="52.85546875"/>
+    <col min="1" max="1" width="102.140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="52.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
@@ -1366,7 +1365,7 @@
         <v>10</v>
       </c>
       <c r="B7" s="18">
-        <v>33.33</v>
+        <v>66.66</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
@@ -1432,7 +1431,7 @@
       <c r="B15" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="C15" s="23" t="s">
+      <c r="C15" s="26" t="s">
         <v>175</v>
       </c>
     </row>
@@ -1443,7 +1442,7 @@
       <c r="B16" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="C16" s="24"/>
+      <c r="C16" s="27"/>
     </row>
     <row r="17" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A17" s="3" t="s">
@@ -1480,112 +1479,112 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="15.7109375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="10.85546875" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="23.5703125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="32.0" collapsed="true"/>
+    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="10.85546875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="23.5703125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="32" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s" s="0">
+      <c r="A1" t="s">
         <v>89</v>
       </c>
-      <c r="B1" t="s" s="0">
+      <c r="B1" t="s">
         <v>90</v>
       </c>
-      <c r="C1" t="s" s="0">
+      <c r="C1" t="s">
         <v>91</v>
       </c>
-      <c r="D1" t="s" s="0">
+      <c r="D1" t="s">
         <v>92</v>
       </c>
-      <c r="E1" t="s" s="0">
+      <c r="E1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s" s="0">
+      <c r="A2" t="s">
         <v>93</v>
       </c>
-      <c r="B2" t="s" s="0">
+      <c r="B2" t="s">
         <v>94</v>
       </c>
-      <c r="C2" t="s" s="0">
+      <c r="C2" t="s">
         <v>95</v>
       </c>
-      <c r="D2" t="s" s="0">
+      <c r="D2" t="s">
         <v>96</v>
       </c>
-      <c r="E2" t="s" s="0">
+      <c r="E2" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s" s="0">
+      <c r="A3" t="s">
         <v>97</v>
       </c>
-      <c r="B3" t="s" s="0">
+      <c r="B3" t="s">
         <v>98</v>
       </c>
-      <c r="C3" t="s" s="0">
+      <c r="C3" t="s">
         <v>99</v>
       </c>
-      <c r="D3" t="s" s="0">
+      <c r="D3" t="s">
         <v>100</v>
       </c>
-      <c r="E3" t="s" s="0">
+      <c r="E3" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s" s="0">
+      <c r="A4" t="s">
         <v>97</v>
       </c>
-      <c r="B4" t="s" s="0">
+      <c r="B4" t="s">
         <v>98</v>
       </c>
-      <c r="C4" t="s" s="0">
+      <c r="C4" t="s">
         <v>101</v>
       </c>
-      <c r="D4" t="s" s="0">
+      <c r="D4" t="s">
         <v>100</v>
       </c>
-      <c r="E4" t="s" s="0">
+      <c r="E4" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s" s="0">
+      <c r="A5" t="s">
         <v>102</v>
       </c>
-      <c r="B5" t="s" s="0">
+      <c r="B5" t="s">
         <v>103</v>
       </c>
-      <c r="C5" t="s" s="0">
+      <c r="C5" t="s">
         <v>104</v>
       </c>
-      <c r="D5" t="s" s="0">
+      <c r="D5" t="s">
         <v>100</v>
       </c>
-      <c r="E5" t="s" s="0">
+      <c r="E5" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s" s="0">
+      <c r="A6" t="s">
         <v>105</v>
       </c>
-      <c r="B6" t="s" s="0">
+      <c r="B6" t="s">
         <v>106</v>
       </c>
-      <c r="C6" t="s" s="0">
+      <c r="C6" t="s">
         <v>107</v>
       </c>
-      <c r="D6" t="s" s="0">
+      <c r="D6" t="s">
         <v>100</v>
       </c>
-      <c r="E6" t="s" s="0">
+      <c r="E6" t="s">
         <v>88</v>
       </c>
     </row>
@@ -1598,37 +1597,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A4B9F6E-5FE6-4DB9-9728-EB3DF1F23798}">
   <dimension ref="A1:K24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="5" width="17.7109375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="1" width="24.28515625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="1" width="21.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="1" width="22.42578125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="21.42578125"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="21.85546875"/>
-    <col min="7" max="7" customWidth="true" width="16.0"/>
-    <col min="9" max="9" customWidth="true" width="12.42578125"/>
-    <col min="11" max="11" customWidth="true" width="11.140625"/>
+    <col min="1" max="1" width="17.7109375" style="5" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="21" style="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="22.42578125" style="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16" customWidth="1"/>
+    <col min="9" max="9" width="12.42578125" customWidth="1"/>
+    <col min="11" max="11" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="28" t="s">
+      <c r="C1" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="28" t="s">
+      <c r="D1" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="26" t="s">
+      <c r="F1" s="23" t="s">
         <v>197</v>
       </c>
     </row>
@@ -1645,7 +1644,7 @@
       <c r="D2" s="8" t="s">
         <v>130</v>
       </c>
-      <c r="F2" t="s" s="0">
+      <c r="F2" t="s">
         <v>198</v>
       </c>
     </row>
@@ -1662,7 +1661,7 @@
       <c r="D3" s="8" t="s">
         <v>133</v>
       </c>
-      <c r="F3" t="s" s="0">
+      <c r="F3" t="s">
         <v>199</v>
       </c>
     </row>
@@ -1679,7 +1678,7 @@
       <c r="D4" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="F4" t="s" s="0">
+      <c r="F4" t="s">
         <v>200</v>
       </c>
     </row>
@@ -1906,18 +1905,18 @@
       <c r="D20" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="F20" s="25" t="s">
+      <c r="F20" s="28" t="s">
         <v>190</v>
       </c>
-      <c r="G20" s="25"/>
-      <c r="H20" s="25" t="s">
+      <c r="G20" s="28"/>
+      <c r="H20" s="28" t="s">
         <v>191</v>
       </c>
-      <c r="I20" s="25"/>
-      <c r="J20" s="25" t="s">
+      <c r="I20" s="28"/>
+      <c r="J20" s="28" t="s">
         <v>192</v>
       </c>
-      <c r="K20" s="25"/>
+      <c r="K20" s="28"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="22" t="s">
@@ -1967,10 +1966,10 @@
       <c r="E22" s="21" t="s">
         <v>172</v>
       </c>
-      <c r="F22" t="s" s="0">
+      <c r="F22" t="s">
         <v>108</v>
       </c>
-      <c r="G22" t="s" s="0">
+      <c r="G22" t="s">
         <v>189</v>
       </c>
       <c r="H22" s="20"/>
@@ -1994,16 +1993,16 @@
       <c r="E23" s="21" t="s">
         <v>195</v>
       </c>
-      <c r="F23" t="s" s="0">
+      <c r="F23" t="s">
         <v>110</v>
       </c>
-      <c r="G23" t="s" s="0">
+      <c r="G23" t="s">
         <v>110</v>
       </c>
-      <c r="H23" t="s" s="0">
+      <c r="H23" t="s">
         <v>110</v>
       </c>
-      <c r="I23" t="s" s="0">
+      <c r="I23" t="s">
         <v>110</v>
       </c>
       <c r="J23" s="20"/>
@@ -2025,22 +2024,22 @@
       <c r="E24" s="21" t="s">
         <v>173</v>
       </c>
-      <c r="F24" t="s" s="0">
+      <c r="F24" t="s">
         <v>108</v>
       </c>
-      <c r="G24" t="s" s="0">
+      <c r="G24" t="s">
         <v>189</v>
       </c>
-      <c r="H24" t="s" s="0">
+      <c r="H24" t="s">
         <v>108</v>
       </c>
-      <c r="I24" t="s" s="0">
+      <c r="I24" t="s">
         <v>189</v>
       </c>
-      <c r="J24" t="s" s="0">
+      <c r="J24" t="s">
         <v>108</v>
       </c>
-      <c r="K24" t="s" s="0">
+      <c r="K24" t="s">
         <v>189</v>
       </c>
     </row>
@@ -2065,16 +2064,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="18.42578125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="21.140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="1" width="9.7109375" collapsed="true"/>
+    <col min="1" max="1" width="18.42578125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="21.140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="9.7109375" style="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s" s="0">
+      <c r="A1" t="s">
         <v>111</v>
       </c>
-      <c r="B1" t="s" s="0">
+      <c r="B1" t="s">
         <v>112</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -2082,10 +2081,10 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s" s="0">
+      <c r="A2" t="s">
         <v>113</v>
       </c>
-      <c r="B2" t="s" s="0">
+      <c r="B2" t="s">
         <v>114</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -2093,10 +2092,10 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s" s="0">
+      <c r="A3" t="s">
         <v>113</v>
       </c>
-      <c r="B3" t="s" s="0">
+      <c r="B3" t="s">
         <v>115</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -2104,10 +2103,10 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s" s="0">
+      <c r="A4" t="s">
         <v>113</v>
       </c>
-      <c r="B4" t="s" s="0">
+      <c r="B4" t="s">
         <v>116</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -2115,10 +2114,10 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s" s="0">
+      <c r="A5" t="s">
         <v>113</v>
       </c>
-      <c r="B5" t="s" s="0">
+      <c r="B5" t="s">
         <v>117</v>
       </c>
       <c r="C5" s="1" t="s">
@@ -2126,10 +2125,10 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s" s="0">
+      <c r="A6" t="s">
         <v>118</v>
       </c>
-      <c r="B6" t="s" s="0">
+      <c r="B6" t="s">
         <v>119</v>
       </c>
       <c r="C6" s="1" t="s">
@@ -2137,10 +2136,10 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s" s="0">
+      <c r="A7" t="s">
         <v>118</v>
       </c>
-      <c r="B7" t="s" s="0">
+      <c r="B7" t="s">
         <v>120</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -2148,10 +2147,10 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s" s="0">
+      <c r="A8" t="s">
         <v>118</v>
       </c>
-      <c r="B8" t="s" s="0">
+      <c r="B8" t="s">
         <v>121</v>
       </c>
       <c r="C8" s="1" t="s">
@@ -2159,10 +2158,10 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s" s="0">
+      <c r="A9" t="s">
         <v>118</v>
       </c>
-      <c r="B9" t="s" s="0">
+      <c r="B9" t="s">
         <v>122</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -2170,10 +2169,10 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s" s="0">
+      <c r="A10" t="s">
         <v>123</v>
       </c>
-      <c r="B10" t="s" s="0">
+      <c r="B10" t="s">
         <v>124</v>
       </c>
       <c r="C10" s="1" t="s">
@@ -2181,10 +2180,10 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s" s="0">
+      <c r="A11" t="s">
         <v>123</v>
       </c>
-      <c r="B11" t="s" s="0">
+      <c r="B11" t="s">
         <v>125</v>
       </c>
       <c r="C11" s="1" t="s">
@@ -2192,10 +2191,10 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s" s="0">
+      <c r="A12" t="s">
         <v>123</v>
       </c>
-      <c r="B12" t="s" s="0">
+      <c r="B12" t="s">
         <v>126</v>
       </c>
       <c r="C12" s="1" t="s">
@@ -2203,10 +2202,10 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s" s="0">
+      <c r="A13" t="s">
         <v>123</v>
       </c>
-      <c r="B13" t="s" s="0">
+      <c r="B13" t="s">
         <v>127</v>
       </c>
       <c r="C13" s="1" t="s">
@@ -2228,16 +2227,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="21.42578125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="25.42578125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="20.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="18.28515625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="17.140625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="19.0" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="11.85546875" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="13.85546875" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="13.140625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
+    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="25.42578125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="20" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="18.28515625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.140625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="19" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="11.85546875" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.85546875" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="13.140625" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -2680,13 +2679,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="19.0"/>
-    <col min="2" max="2" customWidth="true" style="1" width="11.7109375"/>
-    <col min="3" max="3" customWidth="true" style="1" width="21.42578125"/>
+    <col min="1" max="1" width="19" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s" s="0">
+      <c r="A1" t="s">
         <v>59</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -2697,7 +2696,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s" s="0">
+      <c r="A2" t="s">
         <v>62</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -2708,7 +2707,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s" s="0">
+      <c r="A3" t="s">
         <v>65</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -2719,7 +2718,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s" s="0">
+      <c r="A4" t="s">
         <v>65</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -2730,7 +2729,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s" s="0">
+      <c r="A5" t="s">
         <v>65</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -2741,7 +2740,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s" s="0">
+      <c r="A6" t="s">
         <v>65</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -2752,7 +2751,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s" s="0">
+      <c r="A7" t="s">
         <v>65</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -2763,7 +2762,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s" s="0">
+      <c r="A8" t="s">
         <v>75</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -2774,7 +2773,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s" s="0">
+      <c r="A9" t="s">
         <v>77</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -2785,7 +2784,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s" s="0">
+      <c r="A10" t="s">
         <v>80</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -2805,18 +2804,18 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="C5" sqref="C5:E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="23.28515625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="38.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="10.85546875" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="33.0" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="21.7109375" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="21.28515625" collapsed="true"/>
+    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="23.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="38.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="33" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="21.7109375" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="21.28515625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="14" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2865,7 +2864,7 @@
         <v>35</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H2" s="15" t="s">
         <v>35</v>

</xml_diff>

<commit_message>
Four Sanity Flow Completion Update including Refund
</commit_message>
<xml_diff>
--- a/src/test/resources/Sheet/Configsheet.xlsx
+++ b/src/test/resources/Sheet/Configsheet.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jones\eclipse-workspace\Automation-QAPlateron\src\test\resources\Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1FCCA10-9EBD-413B-9697-2990ECAFBAD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B584A99C-91B8-48BB-B235-BFE65D46D594}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="42420" yWindow="0" windowWidth="15180" windowHeight="14040" tabRatio="782" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="782" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill Configuration" sheetId="3" r:id="rId1"/>
-    <sheet name="Employee Details" sheetId="2" r:id="rId2"/>
-    <sheet name="Menu List" sheetId="4" r:id="rId3"/>
-    <sheet name="Modifier List" sheetId="5" r:id="rId4"/>
-    <sheet name="Jobs Configuration" sheetId="1" r:id="rId5"/>
-    <sheet name="Table List" sheetId="6" r:id="rId6"/>
-    <sheet name="Discount" sheetId="7" r:id="rId7"/>
-    <sheet name="Reports" sheetId="8" r:id="rId8"/>
+    <sheet name="Happy Hours" sheetId="9" r:id="rId2"/>
+    <sheet name="Employee Details" sheetId="2" r:id="rId3"/>
+    <sheet name="Menu List" sheetId="4" r:id="rId4"/>
+    <sheet name="Modifier List" sheetId="5" r:id="rId5"/>
+    <sheet name="Jobs Configuration" sheetId="1" r:id="rId6"/>
+    <sheet name="Table List" sheetId="6" r:id="rId7"/>
+    <sheet name="Discount" sheetId="7" r:id="rId8"/>
+    <sheet name="Reports" sheetId="8" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="216">
   <si>
     <t>PhoneNo</t>
   </si>
@@ -708,12 +709,6 @@
     </r>
   </si>
   <si>
-    <t>KfftCvg3df</t>
-  </si>
-  <si>
-    <t>ZzCTLnaaTj</t>
-  </si>
-  <si>
     <t>0.00</t>
   </si>
   <si>
@@ -738,19 +733,70 @@
     <t>Required and Optional</t>
   </si>
   <si>
-    <t>pFiMb9HUdJ</t>
-  </si>
-  <si>
     <t>Cooking Stations Name</t>
   </si>
   <si>
-    <t>Station K6LN9zkLsa</t>
-  </si>
-  <si>
-    <t>Station mBZilaBX33</t>
-  </si>
-  <si>
-    <t>Station xQFyhOvNop</t>
+    <t>22</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>T4</t>
+  </si>
+  <si>
+    <t>T5</t>
+  </si>
+  <si>
+    <t>T6</t>
+  </si>
+  <si>
+    <t>66</t>
+  </si>
+  <si>
+    <t>T8</t>
+  </si>
+  <si>
+    <t>88</t>
+  </si>
+  <si>
+    <t>T9</t>
+  </si>
+  <si>
+    <t>99</t>
+  </si>
+  <si>
+    <t>T10</t>
+  </si>
+  <si>
+    <t>Happy Hour Name</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Total Num of Menus</t>
+  </si>
+  <si>
+    <t>Menus Name &amp; Price</t>
+  </si>
+  <si>
+    <t>z7ifCwMJ5S</t>
+  </si>
+  <si>
+    <t>ALdMdmXESL</t>
+  </si>
+  <si>
+    <t>3cdOx0nngy</t>
+  </si>
+  <si>
+    <t>Station RdBJUegVj2</t>
+  </si>
+  <si>
+    <t>Station uoBygEB9c6</t>
+  </si>
+  <si>
+    <t>Station TMJoVkjLgd</t>
   </si>
 </sst>
 </file>
@@ -992,17 +1038,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1295,7 +1341,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09244190-151A-43A4-A916-8BD3607753C8}">
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" workbookViewId="0">
+    <sheetView zoomScale="70" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -1470,6 +1516,53 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE11A8F6-59E7-43A0-83B7-FC18F6345E4F}">
+  <dimension ref="A1:A5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.140625" style="23" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" customWidth="1"/>
+    <col min="5" max="5" width="20.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="25" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="23" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="24" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="24" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="23" t="s">
+        <v>209</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E6"/>
   <sheetViews>
@@ -1593,7 +1686,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A4B9F6E-5FE6-4DB9-9728-EB3DF1F23798}">
   <dimension ref="A1:K24"/>
   <sheetViews>
@@ -1615,344 +1708,344 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="D1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="23" t="s">
-        <v>197</v>
+      <c r="F1" s="22" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="F2" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="F3" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="F4" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="B2" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="F2" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="22" t="s">
-        <v>186</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>131</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>133</v>
-      </c>
-      <c r="F3" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="22" t="s">
-        <v>186</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="D4" s="8" t="s">
+      <c r="D19" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="F4" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="22" t="s">
-        <v>186</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>137</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>138</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="22" t="s">
-        <v>186</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>139</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="22" t="s">
-        <v>186</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="D7" s="8" t="s">
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="22" t="s">
-        <v>186</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>143</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>144</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="22" t="s">
-        <v>186</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="22" t="s">
-        <v>186</v>
-      </c>
-      <c r="B10" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>148</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="22" t="s">
-        <v>186</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>149</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>150</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="22" t="s">
-        <v>187</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>152</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="22" t="s">
-        <v>187</v>
-      </c>
-      <c r="B13" s="8" t="s">
-        <v>153</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="22" t="s">
-        <v>187</v>
-      </c>
-      <c r="B14" s="8" t="s">
-        <v>154</v>
-      </c>
-      <c r="C14" s="8" t="s">
-        <v>155</v>
-      </c>
-      <c r="D14" s="8" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="22" t="s">
-        <v>187</v>
-      </c>
-      <c r="B15" s="8" t="s">
-        <v>156</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>157</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="22" t="s">
-        <v>187</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>158</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>159</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="22" t="s">
-        <v>187</v>
-      </c>
-      <c r="B17" s="8" t="s">
-        <v>160</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>161</v>
-      </c>
-      <c r="D17" s="8" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="22" t="s">
-        <v>187</v>
-      </c>
-      <c r="B18" s="8" t="s">
-        <v>162</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>163</v>
-      </c>
-      <c r="D18" s="8" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="22" t="s">
-        <v>187</v>
-      </c>
-      <c r="B19" s="8" t="s">
-        <v>164</v>
-      </c>
-      <c r="C19" s="8" t="s">
+      <c r="F20" s="28" t="s">
         <v>188</v>
-      </c>
-      <c r="D19" s="8" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="22" t="s">
-        <v>187</v>
-      </c>
-      <c r="B20" s="8" t="s">
-        <v>165</v>
-      </c>
-      <c r="C20" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="D20" s="8" t="s">
-        <v>136</v>
-      </c>
-      <c r="F20" s="28" t="s">
-        <v>190</v>
       </c>
       <c r="G20" s="28"/>
       <c r="H20" s="28" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="I20" s="28"/>
       <c r="J20" s="28" t="s">
+        <v>190</v>
+      </c>
+      <c r="K20" s="28"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="F21" s="19" t="s">
         <v>192</v>
       </c>
-      <c r="K20" s="28"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="22" t="s">
-        <v>187</v>
-      </c>
-      <c r="B21" s="8" t="s">
-        <v>166</v>
-      </c>
-      <c r="C21" s="8" t="s">
-        <v>167</v>
-      </c>
-      <c r="D21" s="8" t="s">
-        <v>136</v>
-      </c>
-      <c r="F21" s="19" t="s">
-        <v>194</v>
-      </c>
       <c r="G21" s="19" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="H21" s="19" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="I21" s="19" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="J21" s="19" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="K21" s="19" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>196</v>
+        <v>212</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>168</v>
@@ -1970,7 +2063,7 @@
         <v>108</v>
       </c>
       <c r="G22" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="H22" s="20"/>
       <c r="I22" s="20"/>
@@ -1979,7 +2072,7 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>196</v>
+        <v>212</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>169</v>
@@ -1991,7 +2084,7 @@
         <v>130</v>
       </c>
       <c r="E23" s="21" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="F23" t="s">
         <v>110</v>
@@ -2010,7 +2103,7 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>196</v>
+        <v>212</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>170</v>
@@ -2028,19 +2121,19 @@
         <v>108</v>
       </c>
       <c r="G24" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="H24" t="s">
         <v>108</v>
       </c>
       <c r="I24" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="J24" t="s">
         <v>108</v>
       </c>
       <c r="K24" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
   </sheetData>
@@ -2054,7 +2147,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:C13"/>
   <sheetViews>
@@ -2217,7 +2310,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J14"/>
   <sheetViews>
@@ -2669,9 +2762,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{903D10E7-7786-40C4-B45B-1A0F5269C7C8}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A13" sqref="A13"/>
@@ -2711,10 +2804,10 @@
         <v>65</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -2722,10 +2815,10 @@
         <v>65</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -2733,10 +2826,10 @@
         <v>65</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -2755,10 +2848,10 @@
         <v>65</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -2788,10 +2881,109 @@
         <v>80</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>80</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>80</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>80</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>80</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>80</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>80</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C16" s="1" t="s">
         <v>82</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>80</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>80</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>80</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>150</v>
       </c>
     </row>
   </sheetData>
@@ -2799,12 +2991,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA6CF15C-C633-4176-8909-CF9532871AF5}">
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:E5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3014,7 +3206,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB5E0FD6-1845-4CC8-BFCE-C6EAE9737E71}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>